<commit_message>
Created additional code to export the Rule #1 results to the same ticker excel file
</commit_message>
<xml_diff>
--- a/financial_files/excel/AAPL.xlsx
+++ b/financial_files/excel/AAPL.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="financial_data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="financial_data_scraped" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="financial_data" displayName="financial_data" ref="A1:Y119" headerRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="financial_data_scraped" displayName="financial_data_scraped" ref="A1:Y119" headerRowCount="1">
   <autoFilter ref="A1:Y119"/>
   <tableColumns count="25">
     <tableColumn id="1" name="Category"/>

</xml_diff>